<commit_message>
added details in column headers
</commit_message>
<xml_diff>
--- a/supplementary_tables/Table_S5.xlsx
+++ b/supplementary_tables/Table_S5.xlsx
@@ -5,28 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emosca/Google Drive (ettore.mosca.cnr@gmail.com)/FROM_HOME/interactomes/writing/revision/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emosca/Google Drive/FROM_HOME/interactomes/writing/revision2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558D01CA-1689-C44C-B0A7-171D3D63C4A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D33577-F061-1544-84A3-7C28A38EBF7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1320" windowWidth="23220" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="R" sheetId="1" r:id="rId1"/>
-    <sheet name="C_i" sheetId="2" r:id="rId2"/>
-    <sheet name="C_T" sheetId="3" r:id="rId3"/>
-    <sheet name="C_PC" sheetId="5" r:id="rId4"/>
-    <sheet name="C_PATH" sheetId="4" r:id="rId5"/>
-    <sheet name="C_PCT" sheetId="6" r:id="rId6"/>
-    <sheet name="C_DGP" sheetId="7" r:id="rId7"/>
+    <sheet name="Legend" sheetId="8" r:id="rId1"/>
+    <sheet name="R" sheetId="1" r:id="rId2"/>
+    <sheet name="C_I" sheetId="2" r:id="rId3"/>
+    <sheet name="C_T" sheetId="3" r:id="rId4"/>
+    <sheet name="C_PC" sheetId="5" r:id="rId5"/>
+    <sheet name="C_PATH" sheetId="4" r:id="rId6"/>
+    <sheet name="C_PCT" sheetId="6" r:id="rId7"/>
+    <sheet name="C_DGP" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="38">
   <si>
     <t>Topological.centrality.measures</t>
   </si>
@@ -38,9 +39,6 @@
   </si>
   <si>
     <t>Patway.cross.talk</t>
-  </si>
-  <si>
-    <t>NC.disease.gene.analysis</t>
   </si>
   <si>
     <t>BX</t>
@@ -102,13 +100,63 @@
   <si>
     <t>R</t>
   </si>
+  <si>
+    <t>aggregate correlation</t>
+  </si>
+  <si>
+    <t>disease gene prediction</t>
+  </si>
+  <si>
+    <t>C_I</t>
+  </si>
+  <si>
+    <t>weight matrix</t>
+  </si>
+  <si>
+    <t>C_T</t>
+  </si>
+  <si>
+    <t>correlation matrix relative to topological analyses</t>
+  </si>
+  <si>
+    <t>C_PC</t>
+  </si>
+  <si>
+    <t>correlation matrix relative to pathway complexes</t>
+  </si>
+  <si>
+    <t>C_PATH</t>
+  </si>
+  <si>
+    <t>correlation matrix relative to pathways</t>
+  </si>
+  <si>
+    <t>C_PCT</t>
+  </si>
+  <si>
+    <t>C_DGP</t>
+  </si>
+  <si>
+    <t>correlation matrix relative to pathway cross-talk</t>
+  </si>
+  <si>
+    <t>correlation matrix relative to disease gene prioritization</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -136,8 +184,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,470 +500,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5B441D-B9DA-8A47-B2B9-FDC490C50C8E}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0.15</v>
-      </c>
-      <c r="C2">
-        <v>0.53</v>
-      </c>
-      <c r="D2">
-        <v>0.37</v>
-      </c>
-      <c r="E2">
-        <v>0.73</v>
-      </c>
-      <c r="F2">
-        <v>0.19</v>
-      </c>
-      <c r="G2">
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0.27</v>
-      </c>
-      <c r="C3">
-        <v>0.43</v>
-      </c>
-      <c r="D3">
-        <v>0.32</v>
-      </c>
-      <c r="E3">
-        <v>0.74</v>
-      </c>
-      <c r="F3">
-        <v>0.27</v>
-      </c>
-      <c r="G3">
-        <v>2.0300000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0.15</v>
-      </c>
-      <c r="C4">
-        <v>0.5</v>
-      </c>
-      <c r="D4">
-        <v>0.22</v>
-      </c>
-      <c r="E4">
-        <v>0.86</v>
-      </c>
-      <c r="F4">
-        <v>0.2</v>
-      </c>
-      <c r="G4">
-        <v>1.93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0.27</v>
-      </c>
-      <c r="C5">
-        <v>0.59</v>
-      </c>
-      <c r="D5">
-        <v>0.43</v>
-      </c>
-      <c r="E5">
-        <v>0.86</v>
-      </c>
-      <c r="F5">
-        <v>0.35</v>
-      </c>
-      <c r="G5">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>0.43</v>
-      </c>
-      <c r="C6">
-        <v>0.65</v>
-      </c>
-      <c r="D6">
-        <v>0.52</v>
-      </c>
-      <c r="E6">
-        <v>0.85</v>
-      </c>
-      <c r="F6">
-        <v>0.47</v>
-      </c>
-      <c r="G6">
-        <v>2.92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0.51</v>
-      </c>
-      <c r="C7">
-        <v>0.69</v>
-      </c>
-      <c r="D7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E7">
-        <v>0.86</v>
-      </c>
-      <c r="F7">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="G7">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0.43</v>
-      </c>
-      <c r="C8">
-        <v>0.65</v>
-      </c>
-      <c r="D8">
-        <v>0.54</v>
-      </c>
-      <c r="E8">
-        <v>0.83</v>
-      </c>
-      <c r="F8">
-        <v>0.49</v>
-      </c>
-      <c r="G8">
-        <v>2.94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>0.48</v>
-      </c>
-      <c r="C9">
-        <v>0.68</v>
-      </c>
-      <c r="D9">
-        <v>0.59</v>
-      </c>
-      <c r="E9">
-        <v>0.86</v>
-      </c>
-      <c r="F9">
-        <v>0.53</v>
-      </c>
-      <c r="G9">
-        <v>3.14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>0.5</v>
-      </c>
-      <c r="C10">
-        <v>0.69</v>
-      </c>
-      <c r="D10">
-        <v>0.6</v>
-      </c>
-      <c r="E10">
-        <v>0.86</v>
-      </c>
-      <c r="F10">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G10">
-        <v>3.2199999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>0.43</v>
-      </c>
-      <c r="C11">
-        <v>0.64</v>
-      </c>
-      <c r="D11">
-        <v>0.52</v>
-      </c>
-      <c r="E11">
-        <v>0.85</v>
-      </c>
-      <c r="F11">
-        <v>0.46</v>
-      </c>
-      <c r="G11">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>0.5</v>
-      </c>
-      <c r="C12">
-        <v>0.63</v>
-      </c>
-      <c r="D12">
-        <v>0.52</v>
-      </c>
-      <c r="E12">
-        <v>0.86</v>
-      </c>
-      <c r="F12">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G12">
-        <v>3.08</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>0.33</v>
-      </c>
-      <c r="C13">
-        <v>0.54</v>
-      </c>
-      <c r="D13">
-        <v>0.46</v>
-      </c>
-      <c r="E13">
-        <v>0.81</v>
-      </c>
-      <c r="F13">
-        <v>0.4</v>
-      </c>
-      <c r="G13">
-        <v>2.54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>0.5</v>
-      </c>
-      <c r="C14">
-        <v>0.7</v>
-      </c>
-      <c r="D14">
-        <v>0.6</v>
-      </c>
-      <c r="E14">
-        <v>0.86</v>
-      </c>
-      <c r="F14">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G14">
-        <v>3.2199999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>0.33</v>
-      </c>
-      <c r="C15">
-        <v>0.61</v>
-      </c>
-      <c r="D15">
-        <v>0.48</v>
-      </c>
-      <c r="E15">
-        <v>0.84</v>
-      </c>
-      <c r="F15">
-        <v>0.4</v>
-      </c>
-      <c r="G15">
-        <v>2.66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>0.46</v>
-      </c>
-      <c r="C16">
-        <v>0.63</v>
-      </c>
-      <c r="D16">
-        <v>0.52</v>
-      </c>
-      <c r="E16">
-        <v>0.83</v>
-      </c>
-      <c r="F16">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G16">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>0.4</v>
-      </c>
-      <c r="C17">
-        <v>0.45</v>
-      </c>
-      <c r="D17">
-        <v>0.45</v>
-      </c>
-      <c r="E17">
-        <v>0.84</v>
-      </c>
-      <c r="F17">
-        <v>0.44</v>
-      </c>
-      <c r="G17">
-        <v>2.58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>0.36</v>
-      </c>
-      <c r="C18">
-        <v>0.32</v>
-      </c>
-      <c r="D18">
-        <v>0.39</v>
-      </c>
-      <c r="E18">
-        <v>0.84</v>
-      </c>
-      <c r="F18">
-        <v>0.45</v>
-      </c>
-      <c r="G18">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>0.36</v>
-      </c>
-      <c r="C19">
-        <v>0.49</v>
-      </c>
-      <c r="D19">
-        <v>0.47</v>
-      </c>
-      <c r="E19">
-        <v>0.83</v>
-      </c>
-      <c r="F19">
-        <v>0.44</v>
-      </c>
-      <c r="G19">
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <v>0.37</v>
-      </c>
-      <c r="C20">
-        <v>0.41</v>
-      </c>
-      <c r="D20">
-        <v>0.43</v>
-      </c>
-      <c r="E20">
-        <v>0.84</v>
-      </c>
-      <c r="F20">
-        <v>0.42</v>
-      </c>
-      <c r="G20">
-        <v>2.4699999999999998</v>
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -923,6 +574,487 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0.15</v>
+      </c>
+      <c r="C2">
+        <v>0.53</v>
+      </c>
+      <c r="D2">
+        <v>0.37</v>
+      </c>
+      <c r="E2">
+        <v>0.73</v>
+      </c>
+      <c r="F2">
+        <v>0.19</v>
+      </c>
+      <c r="G2">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.27</v>
+      </c>
+      <c r="C3">
+        <v>0.43</v>
+      </c>
+      <c r="D3">
+        <v>0.32</v>
+      </c>
+      <c r="E3">
+        <v>0.74</v>
+      </c>
+      <c r="F3">
+        <v>0.27</v>
+      </c>
+      <c r="G3">
+        <v>2.0300000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.15</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.22</v>
+      </c>
+      <c r="E4">
+        <v>0.86</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.27</v>
+      </c>
+      <c r="C5">
+        <v>0.59</v>
+      </c>
+      <c r="D5">
+        <v>0.43</v>
+      </c>
+      <c r="E5">
+        <v>0.86</v>
+      </c>
+      <c r="F5">
+        <v>0.35</v>
+      </c>
+      <c r="G5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.43</v>
+      </c>
+      <c r="C6">
+        <v>0.65</v>
+      </c>
+      <c r="D6">
+        <v>0.52</v>
+      </c>
+      <c r="E6">
+        <v>0.85</v>
+      </c>
+      <c r="F6">
+        <v>0.47</v>
+      </c>
+      <c r="G6">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.51</v>
+      </c>
+      <c r="C7">
+        <v>0.69</v>
+      </c>
+      <c r="D7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E7">
+        <v>0.86</v>
+      </c>
+      <c r="F7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G7">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.43</v>
+      </c>
+      <c r="C8">
+        <v>0.65</v>
+      </c>
+      <c r="D8">
+        <v>0.54</v>
+      </c>
+      <c r="E8">
+        <v>0.83</v>
+      </c>
+      <c r="F8">
+        <v>0.49</v>
+      </c>
+      <c r="G8">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0.48</v>
+      </c>
+      <c r="C9">
+        <v>0.68</v>
+      </c>
+      <c r="D9">
+        <v>0.59</v>
+      </c>
+      <c r="E9">
+        <v>0.86</v>
+      </c>
+      <c r="F9">
+        <v>0.53</v>
+      </c>
+      <c r="G9">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.69</v>
+      </c>
+      <c r="D10">
+        <v>0.6</v>
+      </c>
+      <c r="E10">
+        <v>0.86</v>
+      </c>
+      <c r="F10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G10">
+        <v>3.2199999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0.43</v>
+      </c>
+      <c r="C11">
+        <v>0.64</v>
+      </c>
+      <c r="D11">
+        <v>0.52</v>
+      </c>
+      <c r="E11">
+        <v>0.85</v>
+      </c>
+      <c r="F11">
+        <v>0.46</v>
+      </c>
+      <c r="G11">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.63</v>
+      </c>
+      <c r="D12">
+        <v>0.52</v>
+      </c>
+      <c r="E12">
+        <v>0.86</v>
+      </c>
+      <c r="F12">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G12">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>0.33</v>
+      </c>
+      <c r="C13">
+        <v>0.54</v>
+      </c>
+      <c r="D13">
+        <v>0.46</v>
+      </c>
+      <c r="E13">
+        <v>0.81</v>
+      </c>
+      <c r="F13">
+        <v>0.4</v>
+      </c>
+      <c r="G13">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>0.7</v>
+      </c>
+      <c r="D14">
+        <v>0.6</v>
+      </c>
+      <c r="E14">
+        <v>0.86</v>
+      </c>
+      <c r="F14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G14">
+        <v>3.2199999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0.33</v>
+      </c>
+      <c r="C15">
+        <v>0.61</v>
+      </c>
+      <c r="D15">
+        <v>0.48</v>
+      </c>
+      <c r="E15">
+        <v>0.84</v>
+      </c>
+      <c r="F15">
+        <v>0.4</v>
+      </c>
+      <c r="G15">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.46</v>
+      </c>
+      <c r="C16">
+        <v>0.63</v>
+      </c>
+      <c r="D16">
+        <v>0.52</v>
+      </c>
+      <c r="E16">
+        <v>0.83</v>
+      </c>
+      <c r="F16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G16">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>0.4</v>
+      </c>
+      <c r="C17">
+        <v>0.45</v>
+      </c>
+      <c r="D17">
+        <v>0.45</v>
+      </c>
+      <c r="E17">
+        <v>0.84</v>
+      </c>
+      <c r="F17">
+        <v>0.44</v>
+      </c>
+      <c r="G17">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>0.36</v>
+      </c>
+      <c r="C18">
+        <v>0.32</v>
+      </c>
+      <c r="D18">
+        <v>0.39</v>
+      </c>
+      <c r="E18">
+        <v>0.84</v>
+      </c>
+      <c r="F18">
+        <v>0.45</v>
+      </c>
+      <c r="G18">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>0.36</v>
+      </c>
+      <c r="C19">
+        <v>0.49</v>
+      </c>
+      <c r="D19">
+        <v>0.47</v>
+      </c>
+      <c r="E19">
+        <v>0.83</v>
+      </c>
+      <c r="F19">
+        <v>0.44</v>
+      </c>
+      <c r="G19">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>0.37</v>
+      </c>
+      <c r="C20">
+        <v>0.41</v>
+      </c>
+      <c r="D20">
+        <v>0.43</v>
+      </c>
+      <c r="E20">
+        <v>0.84</v>
+      </c>
+      <c r="F20">
+        <v>0.42</v>
+      </c>
+      <c r="G20">
+        <v>2.4699999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -934,66 +1066,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1055,7 +1187,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1.88</v>
@@ -1117,7 +1249,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1.95</v>
@@ -1179,7 +1311,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1.93</v>
@@ -1241,7 +1373,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2.09</v>
@@ -1303,7 +1435,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>2.2000000000000002</v>
@@ -1365,7 +1497,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1.83</v>
@@ -1427,7 +1559,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>2.57</v>
@@ -1489,7 +1621,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>2.56</v>
@@ -1551,7 +1683,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>2.08</v>
@@ -1613,7 +1745,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>2.29</v>
@@ -1675,7 +1807,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1.61</v>
@@ -1737,7 +1869,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>2.72</v>
@@ -1799,7 +1931,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1.78</v>
@@ -1861,7 +1993,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1.95</v>
@@ -1923,7 +2055,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>1.52</v>
@@ -1985,7 +2117,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>1.31</v>
@@ -2047,7 +2179,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1.64</v>
@@ -2109,7 +2241,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>1.45</v>
@@ -2174,7 +2306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -2184,66 +2316,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2305,7 +2437,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.03</v>
@@ -2367,7 +2499,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.06</v>
@@ -2429,7 +2561,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>7.0000000000000007E-2</v>
@@ -2491,7 +2623,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -2553,7 +2685,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.21</v>
@@ -2615,7 +2747,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0.09</v>
@@ -2677,7 +2809,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.26</v>
@@ -2739,7 +2871,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.35</v>
@@ -2801,7 +2933,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0.13</v>
@@ -2863,7 +2995,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0.31</v>
@@ -2925,7 +3057,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0.06</v>
@@ -2987,7 +3119,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0.36</v>
@@ -3049,7 +3181,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.05</v>
@@ -3111,7 +3243,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0.19</v>
@@ -3173,7 +3305,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.12</v>
@@ -3235,7 +3367,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0.1</v>
@@ -3297,7 +3429,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0.08</v>
@@ -3359,7 +3491,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0.09</v>
@@ -3424,7 +3556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -3434,66 +3566,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3555,7 +3687,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.44</v>
@@ -3617,7 +3749,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.33</v>
@@ -3679,7 +3811,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.31</v>
@@ -3741,7 +3873,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.47</v>
@@ -3803,7 +3935,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.4</v>
@@ -3865,7 +3997,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0.38</v>
@@ -3927,7 +4059,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.53</v>
@@ -3989,7 +4121,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.43</v>
@@ -4051,7 +4183,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0.41</v>
@@ -4113,7 +4245,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0.36</v>
@@ -4175,7 +4307,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0.28999999999999998</v>
@@ -4237,7 +4369,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0.5</v>
@@ -4299,7 +4431,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.35</v>
@@ -4361,7 +4493,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0.33</v>
@@ -4423,7 +4555,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.27</v>
@@ -4485,7 +4617,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0.19</v>
@@ -4547,7 +4679,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0.34</v>
@@ -4609,7 +4741,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0.26</v>
@@ -4674,7 +4806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -4684,66 +4816,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4805,7 +4937,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.62</v>
@@ -4867,7 +4999,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.64</v>
@@ -4929,7 +5061,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.54</v>
@@ -4991,7 +5123,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.7</v>
@@ -5053,7 +5185,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.62</v>
@@ -5115,7 +5247,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0.56999999999999995</v>
@@ -5177,7 +5309,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.73</v>
@@ -5239,7 +5371,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.64</v>
@@ -5301,7 +5433,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0.66</v>
@@ -5363,7 +5495,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0.53</v>
@@ -5425,7 +5557,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0.48</v>
@@ -5487,7 +5619,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0.68</v>
@@ -5549,7 +5681,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.52</v>
@@ -5611,7 +5743,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0.53</v>
@@ -5673,7 +5805,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.28999999999999998</v>
@@ -5735,7 +5867,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0.15</v>
@@ -5797,7 +5929,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0.36</v>
@@ -5859,7 +5991,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0.25</v>
@@ -5924,7 +6056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
@@ -5934,66 +6066,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6055,7 +6187,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.71</v>
@@ -6117,7 +6249,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.82</v>
@@ -6179,7 +6311,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0.88</v>
@@ -6241,7 +6373,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.72</v>
@@ -6303,7 +6435,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.73</v>
@@ -6365,7 +6497,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0.69</v>
@@ -6427,7 +6559,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.75</v>
@@ -6489,7 +6621,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.73</v>
@@ -6551,7 +6683,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0.74</v>
@@ -6613,7 +6745,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0.73</v>
@@ -6675,7 +6807,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0.69</v>
@@ -6737,7 +6869,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0.74</v>
@@ -6799,7 +6931,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.74</v>
@@ -6861,7 +6993,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0.68</v>
@@ -6923,7 +7055,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.71</v>
@@ -6985,7 +7117,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0.7</v>
@@ -7047,7 +7179,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0.72</v>
@@ -7109,7 +7241,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0.71</v>
@@ -7174,11 +7306,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -7186,66 +7318,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7307,7 +7439,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.09</v>
@@ -7369,7 +7501,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -7431,7 +7563,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0.12</v>
@@ -7493,7 +7625,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -7555,7 +7687,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.24</v>
@@ -7617,7 +7749,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0.11</v>
@@ -7679,7 +7811,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.28999999999999998</v>
@@ -7741,7 +7873,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.41</v>
@@ -7803,7 +7935,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0.14000000000000001</v>
@@ -7865,7 +7997,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0.36</v>
@@ -7927,7 +8059,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0.09</v>
@@ -7989,7 +8121,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0.44</v>
@@ -8051,7 +8183,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.11</v>
@@ -8113,7 +8245,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0.21</v>
@@ -8175,7 +8307,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.14000000000000001</v>
@@ -8237,7 +8369,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>0.16</v>
@@ -8299,7 +8431,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>0.14000000000000001</v>
@@ -8361,7 +8493,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0.15</v>

</xml_diff>